<commit_message>
[ADD] Empezando api + cambios en script
</commit_message>
<xml_diff>
--- a/Normalizacion/Normalizacion.xlsx
+++ b/Normalizacion/Normalizacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bato\p\-SBD1-P1_202202481\Normalizacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A607FC3A-21A5-4F66-AD4B-34945DBFB2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63DACD4-C33A-4100-86E2-5DE7C4E02E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -828,7 +828,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -876,12 +876,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -890,10 +884,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1178,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:P385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+    <sheetView tabSelected="1" topLeftCell="B147" zoomScale="67" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,16 +1253,16 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="22"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -1427,12 +1424,12 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="19"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="16"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -1582,17 +1579,17 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="22"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
@@ -1772,11 +1769,11 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="19"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="23"/>
       <c r="E41" s="16"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1896,12 +1893,12 @@
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C55" s="23"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="19"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="23"/>
       <c r="F55" s="16"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -2039,10 +2036,10 @@
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C71" s="22"/>
+      <c r="C71" s="20"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
@@ -2088,21 +2085,21 @@
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B77" s="24">
+      <c r="B77" s="1">
         <v>5</v>
       </c>
-      <c r="C77" s="24" t="s">
+      <c r="C77" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B85" s="20" t="s">
+      <c r="B85" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="22"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="20"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
@@ -2258,14 +2255,14 @@
     </row>
     <row r="101" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="20" t="s">
+      <c r="B103" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="C103" s="21"/>
-      <c r="D103" s="21"/>
-      <c r="E103" s="21"/>
-      <c r="F103" s="21"/>
-      <c r="G103" s="22"/>
+      <c r="C103" s="19"/>
+      <c r="D103" s="19"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="19"/>
+      <c r="G103" s="20"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B104" s="14" t="s">
@@ -2391,10 +2388,10 @@
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B117" s="18" t="s">
+      <c r="B117" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="C117" s="19"/>
+      <c r="C117" s="23"/>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
@@ -2497,12 +2494,12 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B136" s="20" t="s">
+      <c r="B136" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C136" s="21"/>
-      <c r="D136" s="21"/>
-      <c r="E136" s="22"/>
+      <c r="C136" s="19"/>
+      <c r="D136" s="19"/>
+      <c r="E136" s="20"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B137" s="5" t="s">
@@ -2639,18 +2636,18 @@
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B152" s="20" t="s">
+      <c r="B152" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C152" s="21"/>
-      <c r="D152" s="21"/>
-      <c r="E152" s="21"/>
-      <c r="F152" s="21"/>
-      <c r="G152" s="21"/>
-      <c r="H152" s="21"/>
-      <c r="I152" s="21"/>
-      <c r="J152" s="21"/>
-      <c r="K152" s="22"/>
+      <c r="C152" s="19"/>
+      <c r="D152" s="19"/>
+      <c r="E152" s="19"/>
+      <c r="F152" s="19"/>
+      <c r="G152" s="19"/>
+      <c r="H152" s="19"/>
+      <c r="I152" s="19"/>
+      <c r="J152" s="19"/>
+      <c r="K152" s="20"/>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="s">
@@ -2895,15 +2892,15 @@
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B170" s="18" t="s">
+      <c r="B170" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="C170" s="23"/>
-      <c r="D170" s="23"/>
-      <c r="E170" s="23"/>
-      <c r="F170" s="23"/>
-      <c r="G170" s="23"/>
-      <c r="H170" s="19"/>
+      <c r="C170" s="22"/>
+      <c r="D170" s="22"/>
+      <c r="E170" s="22"/>
+      <c r="F170" s="22"/>
+      <c r="G170" s="22"/>
+      <c r="H170" s="23"/>
       <c r="I170" s="16"/>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.25">
@@ -3048,10 +3045,10 @@
       </c>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B181" s="18" t="s">
+      <c r="B181" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C181" s="19"/>
+      <c r="C181" s="23"/>
       <c r="D181" s="16"/>
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.25">
@@ -3145,13 +3142,13 @@
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B197" s="18" t="s">
+      <c r="B197" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="C197" s="23"/>
-      <c r="D197" s="23"/>
-      <c r="E197" s="23"/>
-      <c r="F197" s="19"/>
+      <c r="C197" s="22"/>
+      <c r="D197" s="22"/>
+      <c r="E197" s="22"/>
+      <c r="F197" s="23"/>
       <c r="G197" s="16"/>
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.25">
@@ -3315,17 +3312,17 @@
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B212" s="18" t="s">
+      <c r="B212" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="C212" s="23"/>
-      <c r="D212" s="23"/>
-      <c r="E212" s="23"/>
-      <c r="F212" s="23"/>
-      <c r="G212" s="23"/>
-      <c r="H212" s="23"/>
-      <c r="I212" s="23"/>
-      <c r="J212" s="19"/>
+      <c r="C212" s="22"/>
+      <c r="D212" s="22"/>
+      <c r="E212" s="22"/>
+      <c r="F212" s="22"/>
+      <c r="G212" s="22"/>
+      <c r="H212" s="22"/>
+      <c r="I212" s="22"/>
+      <c r="J212" s="23"/>
       <c r="K212" s="16"/>
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
@@ -3542,10 +3539,10 @@
       <c r="K221" s="9"/>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B222" s="18" t="s">
+      <c r="B222" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="C222" s="19"/>
+      <c r="C222" s="23"/>
       <c r="D222" s="16"/>
       <c r="E222" s="8"/>
       <c r="F222" s="8"/>
@@ -3673,10 +3670,10 @@
       <c r="K230" s="9"/>
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B231" s="18" t="s">
+      <c r="B231" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="C231" s="19"/>
+      <c r="C231" s="23"/>
       <c r="D231" s="16"/>
       <c r="E231" s="8"/>
       <c r="F231" s="8"/>
@@ -3798,13 +3795,13 @@
       <c r="K239" s="9"/>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B240" s="18" t="s">
+      <c r="B240" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="C240" s="23"/>
-      <c r="D240" s="23"/>
-      <c r="E240" s="23"/>
-      <c r="F240" s="19"/>
+      <c r="C240" s="22"/>
+      <c r="D240" s="22"/>
+      <c r="E240" s="22"/>
+      <c r="F240" s="23"/>
       <c r="G240" s="16"/>
       <c r="H240" s="8"/>
       <c r="I240" s="9"/>
@@ -4055,15 +4052,15 @@
       <c r="L255" s="3"/>
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B258" s="18" t="s">
+      <c r="B258" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="C258" s="23"/>
-      <c r="D258" s="23"/>
-      <c r="E258" s="23"/>
-      <c r="F258" s="23"/>
-      <c r="G258" s="23"/>
-      <c r="H258" s="19"/>
+      <c r="C258" s="22"/>
+      <c r="D258" s="22"/>
+      <c r="E258" s="22"/>
+      <c r="F258" s="22"/>
+      <c r="G258" s="22"/>
+      <c r="H258" s="23"/>
       <c r="I258" s="16"/>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
@@ -4255,12 +4252,12 @@
       </c>
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B276" s="18" t="s">
+      <c r="B276" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="C276" s="23"/>
-      <c r="D276" s="23"/>
-      <c r="E276" s="19"/>
+      <c r="C276" s="22"/>
+      <c r="D276" s="22"/>
+      <c r="E276" s="23"/>
       <c r="F276" s="16"/>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.25">
@@ -4398,16 +4395,16 @@
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B294" s="20" t="s">
+      <c r="B294" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="C294" s="21"/>
-      <c r="D294" s="21"/>
-      <c r="E294" s="21"/>
-      <c r="F294" s="21"/>
-      <c r="G294" s="21"/>
-      <c r="H294" s="21"/>
-      <c r="I294" s="22"/>
+      <c r="C294" s="19"/>
+      <c r="D294" s="19"/>
+      <c r="E294" s="19"/>
+      <c r="F294" s="19"/>
+      <c r="G294" s="19"/>
+      <c r="H294" s="19"/>
+      <c r="I294" s="20"/>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B295" s="1" t="s">
@@ -4616,14 +4613,14 @@
       </c>
     </row>
     <row r="314" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B314" s="20" t="s">
+      <c r="B314" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="C314" s="21"/>
-      <c r="D314" s="21"/>
-      <c r="E314" s="21"/>
-      <c r="F314" s="21"/>
-      <c r="G314" s="22"/>
+      <c r="C314" s="19"/>
+      <c r="D314" s="19"/>
+      <c r="E314" s="19"/>
+      <c r="F314" s="19"/>
+      <c r="G314" s="20"/>
     </row>
     <row r="315" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B315" s="14" t="s">
@@ -4796,14 +4793,14 @@
       </c>
     </row>
     <row r="331" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B331" s="20" t="s">
+      <c r="B331" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="C331" s="21"/>
-      <c r="D331" s="21"/>
-      <c r="E331" s="21"/>
-      <c r="F331" s="21"/>
-      <c r="G331" s="22"/>
+      <c r="C331" s="19"/>
+      <c r="D331" s="19"/>
+      <c r="E331" s="19"/>
+      <c r="F331" s="19"/>
+      <c r="G331" s="20"/>
     </row>
     <row r="332" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B332" s="14" t="s">
@@ -4976,13 +4973,13 @@
       </c>
     </row>
     <row r="348" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B348" s="20" t="s">
+      <c r="B348" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="C348" s="21"/>
-      <c r="D348" s="21"/>
-      <c r="E348" s="21"/>
-      <c r="F348" s="22"/>
+      <c r="C348" s="19"/>
+      <c r="D348" s="19"/>
+      <c r="E348" s="19"/>
+      <c r="F348" s="20"/>
     </row>
     <row r="349" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B349" s="14" t="s">
@@ -5137,13 +5134,13 @@
       </c>
     </row>
     <row r="368" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B368" s="18" t="s">
+      <c r="B368" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="C368" s="23"/>
-      <c r="D368" s="23"/>
-      <c r="E368" s="23"/>
-      <c r="F368" s="19"/>
+      <c r="C368" s="22"/>
+      <c r="D368" s="22"/>
+      <c r="E368" s="22"/>
+      <c r="F368" s="23"/>
       <c r="G368" s="16"/>
     </row>
     <row r="369" spans="1:6" x14ac:dyDescent="0.25">
@@ -5252,13 +5249,13 @@
       </c>
     </row>
     <row r="379" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B379" s="20" t="s">
+      <c r="B379" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="C379" s="21"/>
-      <c r="D379" s="21"/>
-      <c r="E379" s="21"/>
-      <c r="F379" s="22"/>
+      <c r="C379" s="19"/>
+      <c r="D379" s="19"/>
+      <c r="E379" s="19"/>
+      <c r="F379" s="20"/>
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B380" s="1" t="s">
@@ -5367,11 +5364,9 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B331:G331"/>
-    <mergeCell ref="B314:G314"/>
-    <mergeCell ref="B103:G103"/>
-    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B258:H258"/>
+    <mergeCell ref="B276:E276"/>
+    <mergeCell ref="B117:C117"/>
     <mergeCell ref="B85:F85"/>
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="B18:E18"/>
@@ -5379,6 +5374,11 @@
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B55:E55"/>
     <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B331:G331"/>
+    <mergeCell ref="B314:G314"/>
+    <mergeCell ref="B103:G103"/>
+    <mergeCell ref="B379:F379"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B152:K152"/>
     <mergeCell ref="B170:H170"/>
@@ -5390,9 +5390,6 @@
     <mergeCell ref="B222:C222"/>
     <mergeCell ref="B231:C231"/>
     <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B258:H258"/>
-    <mergeCell ref="B276:E276"/>
-    <mergeCell ref="B117:C117"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>